<commit_message>
EPBDS: added new one test for case of using primitive arrays.
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/discriminator/ArrayToArrayCollectionDiscriminatorTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/discriminator/ArrayToArrayCollectionDiscriminatorTest.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>classA</t>
   </si>
@@ -62,9 +62,6 @@
     <t>fieldBDiscriminator</t>
   </si>
   <si>
-    <t>discr1</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -74,27 +71,10 @@
     <t>b.anInteger</t>
   </si>
   <si>
-    <t>Method Object discr2(C source, A[] dest)</t>
-  </si>
-  <si>
-    <t>fieldADiscriminator</t>
-  </si>
-  <si>
-    <t>discr2</t>
-  </si>
-  <si>
-    <t>for (int i = 0; i &lt; dest.length; i++) {
-   if (dest[i].getAString().equals(source.getAString()) ) {
-       return dest[i];
-   }
-}
-return null;</t>
-  </si>
-  <si>
     <t>fieldBType</t>
   </si>
   <si>
-    <t>Method Object discr1(A source, C[] dest)</t>
+    <t>ExternalArrayElementDiscriminator.discriminate</t>
   </si>
 </sst>
 </file>
@@ -198,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -209,10 +189,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C5:J38"/>
+  <dimension ref="C5:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -537,59 +513,57 @@
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10">
-      <c r="C5" s="7" t="s">
+    <row r="5" spans="3:9">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="8" t="s">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="3:9">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="9"/>
+    <row r="7" spans="3:9">
+      <c r="C7" s="7"/>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="9"/>
+    <row r="8" spans="3:9">
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="3:10">
+    <row r="9" spans="3:9">
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="3:10">
+    <row r="10" spans="3:9">
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="3:10">
+    <row r="11" spans="3:9">
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="3:10">
-      <c r="C13" s="10" t="s">
+    <row r="13" spans="3:9">
+      <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="3:10">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="3:9">
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
@@ -606,16 +580,13 @@
         <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="3:10">
+    <row r="15" spans="3:9">
       <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
@@ -632,16 +603,13 @@
         <v>13</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="3:10">
+    <row r="16" spans="3:9">
       <c r="C16" t="s">
         <v>10</v>
       </c>
@@ -658,13 +626,10 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -672,63 +637,22 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" ht="101.25" customHeight="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="2:3" ht="99" customHeight="1">
-      <c r="B4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="102.75" customHeight="1">
-      <c r="B12" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>